<commit_message>
BOJE POMOGIgit add .!
</commit_message>
<xml_diff>
--- a/КопияРейтинг.xlsx
+++ b/КопияРейтинг.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UserProfiles\pr12prohorov.OAT\Desktop\git_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E98D146-EBE0-4626-B7C7-75841659B3D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1A27E2-DEAD-4C90-B973-F981C8821B73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="1080" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,6 +779,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,6 +797,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -806,7 +815,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -823,39 +856,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,22 +1192,22 @@
       <c r="B3" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="23" t="s">
         <v>150</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -1219,7 +1219,7 @@
       <c r="B4" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="24" t="s">
         <v>143</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -1234,7 +1234,7 @@
       <c r="G4" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="23" t="s">
         <v>147</v>
       </c>
       <c r="K4" s="14" t="s">
@@ -1246,7 +1246,7 @@
       <c r="B5" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="24" t="s">
         <v>141</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1261,7 +1261,7 @@
       <c r="G5" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="23" t="s">
         <v>98</v>
       </c>
       <c r="K5" s="14" t="s">
@@ -1273,7 +1273,7 @@
       <c r="B6" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="24" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -1288,7 +1288,7 @@
       <c r="G6" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="23" t="s">
         <v>149</v>
       </c>
       <c r="K6" s="14" t="s">
@@ -1342,15 +1342,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
@@ -1471,15 +1471,15 @@
       <c r="B9" s="12"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -1611,7 +1611,7 @@
   <dimension ref="B2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1633,56 +1633,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="4" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="M4" s="26"/>
+      <c r="M4" s="28"/>
     </row>
     <row r="5" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="5" t="s">
         <v>102</v>
       </c>
@@ -1709,10 +1709,10 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1743,8 +1743,8 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="1" t="s">
         <v>104</v>
       </c>
@@ -1773,8 +1773,8 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="2:13" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1805,8 +1805,8 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="1" t="s">
         <v>106</v>
       </c>
@@ -1835,8 +1835,8 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1865,10 +1865,10 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="34" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1891,8 +1891,8 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1913,8 +1913,8 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1943,8 +1943,8 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="2:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="1" t="s">
         <v>107</v>
       </c>
@@ -1973,8 +1973,8 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
@@ -2003,8 +2003,8 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="2:13" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="1" t="s">
         <v>108</v>
       </c>
@@ -2033,10 +2033,10 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="34" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -2059,8 +2059,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="2" t="s">
         <v>109</v>
       </c>
@@ -2081,8 +2081,8 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
@@ -2103,8 +2103,8 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
@@ -2125,8 +2125,8 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2147,8 +2147,8 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="2:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="34" t="s">
         <v>110</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2167,8 +2167,8 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="2:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="1" t="s">
         <v>112</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="2:13" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="33" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2211,8 +2211,8 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="2:13" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
-      <c r="C25" s="31" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="34" t="s">
         <v>114</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -2235,8 +2235,8 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="2:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="1" t="s">
         <v>116</v>
       </c>
@@ -2257,8 +2257,8 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="2:13" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
-      <c r="C27" s="31" t="s">
+      <c r="B27" s="33"/>
+      <c r="C27" s="34" t="s">
         <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -2277,8 +2277,8 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="1" t="s">
         <v>119</v>
       </c>
@@ -2295,11 +2295,11 @@
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="3">
         <v>38</v>
       </c>
@@ -2326,11 +2326,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B17:B23"/>
@@ -2347,6 +2342,11 @@
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2371,84 +2371,84 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="39" t="s">
+      <c r="B4" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="37"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="34" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="45" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="34"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -2467,8 +2467,8 @@
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
-      <c r="C8" s="38"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="18" t="s">
         <v>18</v>
       </c>
@@ -2485,8 +2485,8 @@
       <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="18" t="s">
         <v>19</v>
       </c>
@@ -2503,8 +2503,8 @@
       <c r="K9" s="18"/>
     </row>
     <row r="10" spans="2:11" ht="51" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="38" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="36" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="18" t="s">
@@ -2523,8 +2523,8 @@
       <c r="K10" s="18"/>
     </row>
     <row r="11" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
@@ -2541,7 +2541,7 @@
       <c r="K11" s="18"/>
     </row>
     <row r="12" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="18" t="s">
         <v>23</v>
       </c>
@@ -2561,8 +2561,8 @@
       <c r="K12" s="18"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="43" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="38" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -2581,8 +2581,8 @@
       <c r="K13" s="18"/>
     </row>
     <row r="14" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="18" t="s">
         <v>27</v>
       </c>
@@ -2599,8 +2599,8 @@
       <c r="K14" s="18"/>
     </row>
     <row r="15" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="18" t="s">
         <v>29</v>
       </c>
@@ -2623,10 +2623,10 @@
       <c r="K15" s="18"/>
     </row>
     <row r="16" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="36" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -2647,8 +2647,8 @@
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="17" t="s">
         <v>33</v>
       </c>
@@ -2667,8 +2667,8 @@
       <c r="K17" s="18"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="17" t="s">
         <v>34</v>
       </c>
@@ -2687,8 +2687,8 @@
       <c r="K18" s="18"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="17" t="s">
         <v>35</v>
       </c>
@@ -2707,8 +2707,8 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="17" t="s">
         <v>36</v>
       </c>
@@ -2727,8 +2727,8 @@
       <c r="K20" s="18"/>
     </row>
     <row r="21" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="38" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="36" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="18" t="s">
@@ -2749,8 +2749,8 @@
       <c r="K21" s="18"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="38"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="18" t="s">
         <v>38</v>
       </c>
@@ -2769,8 +2769,8 @@
       <c r="K22" s="18"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
-      <c r="C23" s="38"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="18" t="s">
         <v>39</v>
       </c>
@@ -2789,8 +2789,8 @@
       <c r="K23" s="18"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="38"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="18" t="s">
         <v>40</v>
       </c>
@@ -2809,8 +2809,8 @@
       <c r="K24" s="18"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="46"/>
-      <c r="C25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="18" t="s">
         <v>41</v>
       </c>
@@ -2829,8 +2829,8 @@
       <c r="K25" s="18"/>
     </row>
     <row r="26" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="46"/>
-      <c r="C26" s="38" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="36" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="17" t="s">
@@ -2851,8 +2851,8 @@
       <c r="K26" s="18"/>
     </row>
     <row r="27" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="46"/>
-      <c r="C27" s="38"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="18" t="s">
         <v>43</v>
       </c>
@@ -2869,8 +2869,8 @@
       <c r="K27" s="18"/>
     </row>
     <row r="28" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="46"/>
-      <c r="C28" s="38"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="18" t="s">
         <v>44</v>
       </c>
@@ -2887,8 +2887,8 @@
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="46"/>
-      <c r="C29" s="38"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="18" t="s">
         <v>45</v>
       </c>
@@ -2907,8 +2907,8 @@
       <c r="K29" s="18"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="46"/>
-      <c r="C30" s="38" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="36" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="18" t="s">
@@ -2927,8 +2927,8 @@
       <c r="K30" s="18"/>
     </row>
     <row r="31" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="46"/>
-      <c r="C31" s="38"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="18" t="s">
         <v>48</v>
       </c>
@@ -2945,8 +2945,8 @@
       <c r="K31" s="18"/>
     </row>
     <row r="32" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="46"/>
-      <c r="C32" s="38"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="18" t="s">
         <v>49</v>
       </c>
@@ -2963,8 +2963,8 @@
       <c r="K32" s="18"/>
     </row>
     <row r="33" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="46"/>
-      <c r="C33" s="38"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="18" t="s">
         <v>134</v>
       </c>
@@ -2981,10 +2981,10 @@
       <c r="K33" s="18"/>
     </row>
     <row r="34" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="36" t="s">
         <v>51</v>
       </c>
       <c r="D34" s="17" t="s">
@@ -3005,8 +3005,8 @@
       <c r="K34" s="18"/>
     </row>
     <row r="35" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="41"/>
-      <c r="C35" s="38"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="17" t="s">
         <v>53</v>
       </c>
@@ -3023,8 +3023,8 @@
       <c r="K35" s="18"/>
     </row>
     <row r="36" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="41"/>
-      <c r="C36" s="38"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="17" t="s">
         <v>54</v>
       </c>
@@ -3041,8 +3041,8 @@
       <c r="K36" s="18"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="41"/>
-      <c r="C37" s="38"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="17" t="s">
         <v>55</v>
       </c>
@@ -3059,8 +3059,8 @@
       <c r="K37" s="18"/>
     </row>
     <row r="38" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="41"/>
-      <c r="C38" s="38"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="17" t="s">
         <v>56</v>
       </c>
@@ -3077,8 +3077,8 @@
       <c r="K38" s="18"/>
     </row>
     <row r="39" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="41"/>
-      <c r="C39" s="38"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="18" t="s">
         <v>57</v>
       </c>
@@ -3097,8 +3097,8 @@
       <c r="K39" s="18"/>
     </row>
     <row r="40" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="41"/>
-      <c r="C40" s="38"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="18" t="s">
         <v>58</v>
       </c>
@@ -3115,8 +3115,8 @@
       <c r="K40" s="18"/>
     </row>
     <row r="41" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="41"/>
-      <c r="C41" s="43" t="s">
+      <c r="B41" s="42"/>
+      <c r="C41" s="38" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="17" t="s">
@@ -3137,8 +3137,8 @@
       <c r="K41" s="18"/>
     </row>
     <row r="42" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="41"/>
-      <c r="C42" s="44"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="18" t="s">
         <v>61</v>
       </c>
@@ -3157,8 +3157,8 @@
       <c r="K42" s="18"/>
     </row>
     <row r="43" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="41"/>
-      <c r="C43" s="45"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="18" t="s">
         <v>62</v>
       </c>
@@ -3177,8 +3177,8 @@
       <c r="K43" s="18"/>
     </row>
     <row r="44" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="41"/>
-      <c r="C44" s="38" t="s">
+      <c r="B44" s="42"/>
+      <c r="C44" s="36" t="s">
         <v>63</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -3197,8 +3197,8 @@
       <c r="K44" s="18"/>
     </row>
     <row r="45" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="41"/>
-      <c r="C45" s="38"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="18" t="s">
         <v>65</v>
       </c>
@@ -3215,8 +3215,8 @@
       <c r="K45" s="18"/>
     </row>
     <row r="46" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="41"/>
-      <c r="C46" s="38"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="18" t="s">
         <v>66</v>
       </c>
@@ -3233,8 +3233,8 @@
       <c r="K46" s="18"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="41"/>
-      <c r="C47" s="38"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="18" t="s">
         <v>92</v>
       </c>
@@ -3253,8 +3253,8 @@
       <c r="K47" s="18"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="41"/>
-      <c r="C48" s="38"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="18" t="s">
         <v>67</v>
       </c>
@@ -3273,8 +3273,8 @@
       <c r="K48" s="18"/>
     </row>
     <row r="49" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="41"/>
-      <c r="C49" s="38"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="36"/>
       <c r="D49" s="18" t="s">
         <v>68</v>
       </c>
@@ -3293,8 +3293,8 @@
       <c r="K49" s="18"/>
     </row>
     <row r="50" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="41"/>
-      <c r="C50" s="43" t="s">
+      <c r="B50" s="42"/>
+      <c r="C50" s="38" t="s">
         <v>69</v>
       </c>
       <c r="D50" s="18" t="s">
@@ -3315,8 +3315,8 @@
       <c r="K50" s="18"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="41"/>
-      <c r="C51" s="44"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="39"/>
       <c r="D51" s="18" t="s">
         <v>82</v>
       </c>
@@ -3335,8 +3335,8 @@
       <c r="K51" s="18"/>
     </row>
     <row r="52" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="41"/>
-      <c r="C52" s="44"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="39"/>
       <c r="D52" s="18" t="s">
         <v>133</v>
       </c>
@@ -3355,8 +3355,8 @@
       <c r="K52" s="18"/>
     </row>
     <row r="53" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B53" s="41"/>
-      <c r="C53" s="44"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="39"/>
       <c r="D53" s="18" t="s">
         <v>83</v>
       </c>
@@ -3373,8 +3373,8 @@
       <c r="K53" s="18"/>
     </row>
     <row r="54" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="41"/>
-      <c r="C54" s="44"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="18" t="s">
         <v>84</v>
       </c>
@@ -3391,8 +3391,8 @@
       <c r="K54" s="18"/>
     </row>
     <row r="55" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="41"/>
-      <c r="C55" s="44"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="18" t="s">
         <v>85</v>
       </c>
@@ -3409,8 +3409,8 @@
       <c r="K55" s="18"/>
     </row>
     <row r="56" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="41"/>
-      <c r="C56" s="44"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="39"/>
       <c r="D56" s="18" t="s">
         <v>86</v>
       </c>
@@ -3427,8 +3427,8 @@
       <c r="K56" s="18"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="42"/>
-      <c r="C57" s="45"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="40"/>
       <c r="D57" s="18" t="s">
         <v>93</v>
       </c>
@@ -3469,10 +3469,10 @@
       <c r="K58" s="18"/>
     </row>
     <row r="59" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="43" t="s">
+      <c r="C59" s="38" t="s">
         <v>73</v>
       </c>
       <c r="D59" s="18" t="s">
@@ -3491,8 +3491,8 @@
       <c r="K59" s="18"/>
     </row>
     <row r="60" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B60" s="41"/>
-      <c r="C60" s="44"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="39"/>
       <c r="D60" s="18" t="s">
         <v>75</v>
       </c>
@@ -3509,8 +3509,8 @@
       <c r="K60" s="18"/>
     </row>
     <row r="61" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="41"/>
-      <c r="C61" s="45"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="40"/>
       <c r="D61" s="18" t="s">
         <v>76</v>
       </c>
@@ -3527,8 +3527,8 @@
       <c r="K61" s="18"/>
     </row>
     <row r="62" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="41"/>
-      <c r="C62" s="43" t="s">
+      <c r="B62" s="42"/>
+      <c r="C62" s="38" t="s">
         <v>77</v>
       </c>
       <c r="D62" s="18" t="s">
@@ -3547,8 +3547,8 @@
       <c r="K62" s="18"/>
     </row>
     <row r="63" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="41"/>
-      <c r="C63" s="45"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="40"/>
       <c r="D63" s="18" t="s">
         <v>79</v>
       </c>
@@ -3565,10 +3565,10 @@
       <c r="K63" s="18"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="43" t="s">
+      <c r="C64" s="38" t="s">
         <v>122</v>
       </c>
       <c r="D64" s="18" t="s">
@@ -3593,8 +3593,8 @@
       <c r="K64" s="18"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="41"/>
-      <c r="C65" s="44"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="39"/>
       <c r="D65" s="18" t="s">
         <v>124</v>
       </c>
@@ -3617,8 +3617,8 @@
       <c r="K65" s="18"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="41"/>
-      <c r="C66" s="44"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="39"/>
       <c r="D66" s="18" t="s">
         <v>125</v>
       </c>
@@ -3641,8 +3641,8 @@
       <c r="K66" s="18"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="42"/>
-      <c r="C67" s="45"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="18" t="s">
         <v>126</v>
       </c>
@@ -3665,11 +3665,11 @@
       <c r="K67" s="18"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="39" t="s">
+      <c r="B68" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
       <c r="E68" s="17">
         <f>SUM(E7:E67)</f>
         <v>70</v>
@@ -3695,6 +3695,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B34:B57"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B7:B15"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D4:D6"/>
@@ -3711,21 +3726,6 @@
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C59:C61"/>
     <mergeCell ref="B59:B63"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="B34:B57"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B7:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>